<commit_message>
Proquest Orthographic Consistency sift completed
</commit_message>
<xml_diff>
--- a/Reading_list_abstract_sift.xlsx
+++ b/Reading_list_abstract_sift.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" tabRatio="500"/>
+    <workbookView xWindow="13400" yWindow="460" windowWidth="21420" windowHeight="18940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3308" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4141" uniqueCount="598">
   <si>
     <t>Study (R / Q)</t>
   </si>
@@ -1617,6 +1617,210 @@
   </si>
   <si>
     <t>Anne Cunningham</t>
+  </si>
+  <si>
+    <t>Predicting reading comprehension of narrative and expository texts among Hebrew-speaking readers with and without a reading disability</t>
+  </si>
+  <si>
+    <t>linkage study</t>
+  </si>
+  <si>
+    <t>developmental surface and phonological dysgraphia in German 3rd Graders</t>
+  </si>
+  <si>
+    <t>Park Jungjun</t>
+  </si>
+  <si>
+    <t>Linda J Lombardino</t>
+  </si>
+  <si>
+    <t>Characteristics of phonological processing, reading, oral language and auditory processing skills of children with mild-to-moderate SN Hearing Loss</t>
+  </si>
+  <si>
+    <t>No item effects</t>
+  </si>
+  <si>
+    <t>sublexical frequency measures for orthographical and phonological units in German</t>
+  </si>
+  <si>
+    <t>Locus and Nature of perceptual phonological deficity in Spanish Children with Reading Disabilities</t>
+  </si>
+  <si>
+    <t>Spelling consistency affects reading in Young Dutch readers with and without Dyslexia</t>
+  </si>
+  <si>
+    <t>Gene P Oulette</t>
+  </si>
+  <si>
+    <t>Carelton University Canada</t>
+  </si>
+  <si>
+    <t>Pathways to literacy:   A study of invented spelling and its role in learning to read</t>
+  </si>
+  <si>
+    <t>Auditory modality</t>
+  </si>
+  <si>
+    <t>spelling</t>
+  </si>
+  <si>
+    <t>Auditory word identification and phonological skills in dyslexic and average readers</t>
+  </si>
+  <si>
+    <t>Explicit and implicit processing of words and pseudowords by adult developmental dyslexics: A search for Wernicke's Wortschatz?</t>
+  </si>
+  <si>
+    <t>management</t>
+  </si>
+  <si>
+    <t>writing study</t>
+  </si>
+  <si>
+    <t>music study</t>
+  </si>
+  <si>
+    <t>grapheme analysis</t>
+  </si>
+  <si>
+    <t>The impact of fading reading on children with reading difficulties</t>
+  </si>
+  <si>
+    <t>genetic study</t>
+  </si>
+  <si>
+    <t>a comparison of orthographic processing in children with and without reading and spelling disorder in a regular orthography</t>
+  </si>
+  <si>
+    <t>The effects of orthographic transparency and familiarity on reading Hebrew words in adults with and without  dyslexia</t>
+  </si>
+  <si>
+    <t>opinion article</t>
+  </si>
+  <si>
+    <t>Phonological awareness and reading in Children with and without Dyslexia in English and Kannada</t>
+  </si>
+  <si>
+    <t>Eye movements of university students with and without reading difficulties during naming speed tasks</t>
+  </si>
+  <si>
+    <t>Individual Differences in Reading Development: A review of 25 years of Empirical Research on Matthew Effects on Reading</t>
+  </si>
+  <si>
+    <t>written in Spanish</t>
+  </si>
+  <si>
+    <t>Individual differences in children's literacy development: the contribution of orthographic knowledge</t>
+  </si>
+  <si>
+    <t>The  double deficit hypothesis in the transparent Finnish  orthography: a longitudinal study from Kindergarten to Grade 2</t>
+  </si>
+  <si>
+    <t>Improving word  reading speed: individual differences interact with a training focus on successes or failures</t>
+  </si>
+  <si>
+    <t>dyslexia review</t>
+  </si>
+  <si>
+    <t>advertising</t>
+  </si>
+  <si>
+    <t>Orthographic influences on sublexical processing</t>
+  </si>
+  <si>
+    <t>Rachael Suddarth</t>
+  </si>
+  <si>
+    <t>Elena Plante</t>
+  </si>
+  <si>
+    <t>Naming speed and reading: from prediction to instruction</t>
+  </si>
+  <si>
+    <t>dyslexia study</t>
+  </si>
+  <si>
+    <t>Changes in reading strategies in school age children</t>
+  </si>
+  <si>
+    <t>Variability in reading ability</t>
+  </si>
+  <si>
+    <t>John Adam Naples</t>
+  </si>
+  <si>
+    <t>Elena L Grigorenko</t>
+  </si>
+  <si>
+    <t>Yale University</t>
+  </si>
+  <si>
+    <t>Evaluation of the double deficit hypothesis subtype classification of readers in Spanish</t>
+  </si>
+  <si>
+    <t>Computer speech-based remediation for RD: The size of spelling to sound unit in a transparent orthography</t>
+  </si>
+  <si>
+    <t>Evaluating the procedural deficit hypothesis: Language and motor deficits in preschool children</t>
+  </si>
+  <si>
+    <t>Renee Laura Fabus</t>
+  </si>
+  <si>
+    <t>Colombia University</t>
+  </si>
+  <si>
+    <t>Core deficits and variable differences in Dutch poor readers learning English</t>
+  </si>
+  <si>
+    <t>Dyslexia and dysgraphia in Greek in relation to normal development: Cross linguistic and longitudinal studies</t>
+  </si>
+  <si>
+    <t>Vassiliki Diamanti</t>
+  </si>
+  <si>
+    <t>University college London</t>
+  </si>
+  <si>
+    <t>is the deficit in phonological awareness better explained in terms of task differences or effects of syllable structure</t>
+  </si>
+  <si>
+    <t>Lexical access in children with reading disorder: The lexical indeterminy hypothesis</t>
+  </si>
+  <si>
+    <t>David D Schwartz</t>
+  </si>
+  <si>
+    <t>Brian P Ackerman</t>
+  </si>
+  <si>
+    <t>University of Delaware</t>
+  </si>
+  <si>
+    <t>animal study</t>
+  </si>
+  <si>
+    <t>Multiple pathways to dysfluent reading: a developmental-componential investigation of the development and breakdown of fluent reading</t>
+  </si>
+  <si>
+    <t>Tami Katzir</t>
+  </si>
+  <si>
+    <t>A developmental profile of reading errors in disabled and normal readers</t>
+  </si>
+  <si>
+    <t>janet louise Henderson</t>
+  </si>
+  <si>
+    <t>Linda Siegel</t>
+  </si>
+  <si>
+    <t>Janet Margaret Olds</t>
+  </si>
+  <si>
+    <t>McMaster University, Canada</t>
+  </si>
+  <si>
+    <t>Reading and repetition individual differences in adult reading skill</t>
   </si>
 </sst>
 </file>
@@ -1973,23 +2177,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W656"/>
+  <dimension ref="A1:W863"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="210" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A643" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D656" sqref="D656"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="210" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A848" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D848" sqref="D848:D859"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="3" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="46.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="24.33203125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="16.5" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="13.5" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="21.1640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="21.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" style="1" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21.6640625" customWidth="1"/>
     <col min="17" max="17" width="21.5" bestFit="1" customWidth="1"/>
@@ -15796,6 +16001,15 @@
       </c>
     </row>
     <row r="622" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A622">
+        <v>8</v>
+      </c>
+      <c r="B622" t="s">
+        <v>129</v>
+      </c>
+      <c r="C622" t="s">
+        <v>507</v>
+      </c>
       <c r="D622" s="1" t="s">
         <v>509</v>
       </c>
@@ -15807,6 +16021,15 @@
       </c>
     </row>
     <row r="623" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A623">
+        <v>8</v>
+      </c>
+      <c r="B623" t="s">
+        <v>129</v>
+      </c>
+      <c r="C623" t="s">
+        <v>507</v>
+      </c>
       <c r="D623" s="1" t="s">
         <v>510</v>
       </c>
@@ -15821,6 +16044,15 @@
       </c>
     </row>
     <row r="624" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A624">
+        <v>8</v>
+      </c>
+      <c r="B624" t="s">
+        <v>129</v>
+      </c>
+      <c r="C624" t="s">
+        <v>507</v>
+      </c>
       <c r="D624" s="1" t="s">
         <v>357</v>
       </c>
@@ -15831,7 +16063,16 @@
         <v>262</v>
       </c>
     </row>
-    <row r="625" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="625" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A625">
+        <v>8</v>
+      </c>
+      <c r="B625" t="s">
+        <v>129</v>
+      </c>
+      <c r="C625" t="s">
+        <v>507</v>
+      </c>
       <c r="D625" s="1">
         <v>6</v>
       </c>
@@ -15842,7 +16083,19 @@
         <v>49</v>
       </c>
     </row>
-    <row r="626" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="626" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A626">
+        <v>8</v>
+      </c>
+      <c r="B626" t="s">
+        <v>129</v>
+      </c>
+      <c r="C626" t="s">
+        <v>507</v>
+      </c>
+      <c r="D626" s="1">
+        <v>7</v>
+      </c>
       <c r="L626" t="s">
         <v>194</v>
       </c>
@@ -15850,7 +16103,19 @@
         <v>432</v>
       </c>
     </row>
-    <row r="627" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="627" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A627">
+        <v>8</v>
+      </c>
+      <c r="B627" t="s">
+        <v>129</v>
+      </c>
+      <c r="C627" t="s">
+        <v>507</v>
+      </c>
+      <c r="D627" s="1">
+        <v>8</v>
+      </c>
       <c r="L627" t="s">
         <v>46</v>
       </c>
@@ -15858,7 +16123,19 @@
         <v>197</v>
       </c>
     </row>
-    <row r="628" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="628" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A628">
+        <v>8</v>
+      </c>
+      <c r="B628" t="s">
+        <v>129</v>
+      </c>
+      <c r="C628" t="s">
+        <v>507</v>
+      </c>
+      <c r="D628" s="1">
+        <v>9</v>
+      </c>
       <c r="L628" t="s">
         <v>46</v>
       </c>
@@ -15866,7 +16143,16 @@
         <v>57</v>
       </c>
     </row>
-    <row r="629" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="629" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A629">
+        <v>8</v>
+      </c>
+      <c r="B629" t="s">
+        <v>129</v>
+      </c>
+      <c r="C629" t="s">
+        <v>507</v>
+      </c>
       <c r="D629" s="1" t="s">
         <v>514</v>
       </c>
@@ -15898,7 +16184,16 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="630" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="630" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A630">
+        <v>8</v>
+      </c>
+      <c r="B630" t="s">
+        <v>129</v>
+      </c>
+      <c r="C630" t="s">
+        <v>507</v>
+      </c>
       <c r="D630" s="1" t="s">
         <v>302</v>
       </c>
@@ -15909,7 +16204,16 @@
         <v>262</v>
       </c>
     </row>
-    <row r="631" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="631" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A631">
+        <v>8</v>
+      </c>
+      <c r="B631" t="s">
+        <v>129</v>
+      </c>
+      <c r="C631" t="s">
+        <v>507</v>
+      </c>
       <c r="D631" s="1">
         <v>12</v>
       </c>
@@ -15920,7 +16224,19 @@
         <v>515</v>
       </c>
     </row>
-    <row r="632" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="632" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A632">
+        <v>8</v>
+      </c>
+      <c r="B632" t="s">
+        <v>129</v>
+      </c>
+      <c r="C632" t="s">
+        <v>507</v>
+      </c>
+      <c r="D632" s="1">
+        <v>13</v>
+      </c>
       <c r="L632" t="s">
         <v>46</v>
       </c>
@@ -15928,7 +16244,19 @@
         <v>49</v>
       </c>
     </row>
-    <row r="633" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="633" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A633">
+        <v>8</v>
+      </c>
+      <c r="B633" t="s">
+        <v>129</v>
+      </c>
+      <c r="C633" t="s">
+        <v>507</v>
+      </c>
+      <c r="D633" s="1">
+        <v>14</v>
+      </c>
       <c r="L633" t="s">
         <v>46</v>
       </c>
@@ -15936,7 +16264,19 @@
         <v>515</v>
       </c>
     </row>
-    <row r="634" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="634" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A634">
+        <v>8</v>
+      </c>
+      <c r="B634" t="s">
+        <v>129</v>
+      </c>
+      <c r="C634" t="s">
+        <v>507</v>
+      </c>
+      <c r="D634" s="1">
+        <v>15</v>
+      </c>
       <c r="L634" t="s">
         <v>46</v>
       </c>
@@ -15944,7 +16284,16 @@
         <v>196</v>
       </c>
     </row>
-    <row r="635" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="635" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A635">
+        <v>8</v>
+      </c>
+      <c r="B635" t="s">
+        <v>129</v>
+      </c>
+      <c r="C635" t="s">
+        <v>507</v>
+      </c>
       <c r="D635" s="1" t="s">
         <v>308</v>
       </c>
@@ -15973,7 +16322,16 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="636" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="636" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A636">
+        <v>8</v>
+      </c>
+      <c r="B636" t="s">
+        <v>129</v>
+      </c>
+      <c r="C636" t="s">
+        <v>507</v>
+      </c>
       <c r="D636" s="1">
         <v>17</v>
       </c>
@@ -15984,7 +16342,16 @@
         <v>55</v>
       </c>
     </row>
-    <row r="637" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="637" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A637">
+        <v>8</v>
+      </c>
+      <c r="B637" t="s">
+        <v>129</v>
+      </c>
+      <c r="C637" t="s">
+        <v>507</v>
+      </c>
       <c r="D637" s="1" t="s">
         <v>517</v>
       </c>
@@ -16016,7 +16383,16 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="638" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="638" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A638">
+        <v>8</v>
+      </c>
+      <c r="B638" t="s">
+        <v>129</v>
+      </c>
+      <c r="C638" t="s">
+        <v>507</v>
+      </c>
       <c r="D638" s="1">
         <v>19</v>
       </c>
@@ -16027,7 +16403,19 @@
         <v>520</v>
       </c>
     </row>
-    <row r="639" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="639" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A639">
+        <v>8</v>
+      </c>
+      <c r="B639" t="s">
+        <v>129</v>
+      </c>
+      <c r="C639" t="s">
+        <v>507</v>
+      </c>
+      <c r="D639" s="1">
+        <v>20</v>
+      </c>
       <c r="L639" t="s">
         <v>46</v>
       </c>
@@ -16035,7 +16423,16 @@
         <v>515</v>
       </c>
     </row>
-    <row r="640" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="640" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A640">
+        <v>8</v>
+      </c>
+      <c r="B640" t="s">
+        <v>129</v>
+      </c>
+      <c r="C640" t="s">
+        <v>507</v>
+      </c>
       <c r="D640" s="1" t="s">
         <v>521</v>
       </c>
@@ -16046,7 +16443,16 @@
         <v>262</v>
       </c>
     </row>
-    <row r="641" spans="4:20" ht="48" x14ac:dyDescent="0.2">
+    <row r="641" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A641">
+        <v>8</v>
+      </c>
+      <c r="B641" t="s">
+        <v>129</v>
+      </c>
+      <c r="C641" t="s">
+        <v>507</v>
+      </c>
       <c r="D641" s="1" t="s">
         <v>522</v>
       </c>
@@ -16054,7 +16460,16 @@
         <v>69</v>
       </c>
     </row>
-    <row r="642" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="642" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A642">
+        <v>8</v>
+      </c>
+      <c r="B642" t="s">
+        <v>129</v>
+      </c>
+      <c r="C642" t="s">
+        <v>507</v>
+      </c>
       <c r="D642" s="1">
         <v>23</v>
       </c>
@@ -16065,7 +16480,16 @@
         <v>515</v>
       </c>
     </row>
-    <row r="643" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="643" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A643">
+        <v>8</v>
+      </c>
+      <c r="B643" t="s">
+        <v>129</v>
+      </c>
+      <c r="C643" t="s">
+        <v>507</v>
+      </c>
       <c r="D643" s="1">
         <v>24</v>
       </c>
@@ -16076,7 +16500,16 @@
         <v>57</v>
       </c>
     </row>
-    <row r="644" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="644" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A644">
+        <v>8</v>
+      </c>
+      <c r="B644" t="s">
+        <v>129</v>
+      </c>
+      <c r="C644" t="s">
+        <v>507</v>
+      </c>
       <c r="D644" s="1">
         <v>25</v>
       </c>
@@ -16087,7 +16520,16 @@
         <v>515</v>
       </c>
     </row>
-    <row r="645" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="645" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A645">
+        <v>8</v>
+      </c>
+      <c r="B645" t="s">
+        <v>129</v>
+      </c>
+      <c r="C645" t="s">
+        <v>507</v>
+      </c>
       <c r="D645" s="1">
         <v>26</v>
       </c>
@@ -16098,7 +16540,16 @@
         <v>523</v>
       </c>
     </row>
-    <row r="646" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="646" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A646">
+        <v>8</v>
+      </c>
+      <c r="B646" t="s">
+        <v>129</v>
+      </c>
+      <c r="C646" t="s">
+        <v>507</v>
+      </c>
       <c r="D646" s="1">
         <v>27</v>
       </c>
@@ -16109,7 +16560,16 @@
         <v>515</v>
       </c>
     </row>
-    <row r="647" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="647" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A647">
+        <v>8</v>
+      </c>
+      <c r="B647" t="s">
+        <v>129</v>
+      </c>
+      <c r="C647" t="s">
+        <v>507</v>
+      </c>
       <c r="D647" s="1">
         <v>28</v>
       </c>
@@ -16120,7 +16580,16 @@
         <v>55</v>
       </c>
     </row>
-    <row r="648" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="648" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A648">
+        <v>8</v>
+      </c>
+      <c r="B648" t="s">
+        <v>129</v>
+      </c>
+      <c r="C648" t="s">
+        <v>507</v>
+      </c>
       <c r="D648" s="1">
         <v>29</v>
       </c>
@@ -16131,7 +16600,16 @@
         <v>515</v>
       </c>
     </row>
-    <row r="649" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="649" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A649">
+        <v>8</v>
+      </c>
+      <c r="B649" t="s">
+        <v>129</v>
+      </c>
+      <c r="C649" t="s">
+        <v>507</v>
+      </c>
       <c r="D649" s="1">
         <v>30</v>
       </c>
@@ -16142,7 +16620,16 @@
         <v>55</v>
       </c>
     </row>
-    <row r="650" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="650" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A650">
+        <v>8</v>
+      </c>
+      <c r="B650" t="s">
+        <v>129</v>
+      </c>
+      <c r="C650" t="s">
+        <v>507</v>
+      </c>
       <c r="D650" s="1">
         <v>31</v>
       </c>
@@ -16153,7 +16640,16 @@
         <v>55</v>
       </c>
     </row>
-    <row r="651" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="651" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A651">
+        <v>8</v>
+      </c>
+      <c r="B651" t="s">
+        <v>129</v>
+      </c>
+      <c r="C651" t="s">
+        <v>507</v>
+      </c>
       <c r="D651" s="1">
         <v>32</v>
       </c>
@@ -16164,7 +16660,16 @@
         <v>523</v>
       </c>
     </row>
-    <row r="652" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="652" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A652">
+        <v>8</v>
+      </c>
+      <c r="B652" t="s">
+        <v>129</v>
+      </c>
+      <c r="C652" t="s">
+        <v>507</v>
+      </c>
       <c r="D652" s="1" t="s">
         <v>524</v>
       </c>
@@ -16193,7 +16698,16 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="653" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="653" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A653">
+        <v>8</v>
+      </c>
+      <c r="B653" t="s">
+        <v>129</v>
+      </c>
+      <c r="C653" t="s">
+        <v>507</v>
+      </c>
       <c r="D653" s="1">
         <v>34</v>
       </c>
@@ -16204,7 +16718,16 @@
         <v>515</v>
       </c>
     </row>
-    <row r="654" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="654" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A654">
+        <v>8</v>
+      </c>
+      <c r="B654" t="s">
+        <v>129</v>
+      </c>
+      <c r="C654" t="s">
+        <v>507</v>
+      </c>
       <c r="D654" s="1">
         <v>35</v>
       </c>
@@ -16215,7 +16738,16 @@
         <v>57</v>
       </c>
     </row>
-    <row r="655" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="655" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A655">
+        <v>8</v>
+      </c>
+      <c r="B655" t="s">
+        <v>129</v>
+      </c>
+      <c r="C655" t="s">
+        <v>507</v>
+      </c>
       <c r="D655" s="1" t="s">
         <v>527</v>
       </c>
@@ -16244,9 +16776,3597 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="656" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="656" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A656">
+        <v>8</v>
+      </c>
+      <c r="B656" t="s">
+        <v>129</v>
+      </c>
+      <c r="C656" t="s">
+        <v>507</v>
+      </c>
       <c r="D656" s="1">
         <v>37</v>
+      </c>
+      <c r="L656" t="s">
+        <v>194</v>
+      </c>
+      <c r="M656" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="657" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A657">
+        <v>8</v>
+      </c>
+      <c r="B657" t="s">
+        <v>129</v>
+      </c>
+      <c r="C657" t="s">
+        <v>507</v>
+      </c>
+      <c r="D657" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="L657" t="s">
+        <v>69</v>
+      </c>
+      <c r="N657" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="658" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A658">
+        <v>8</v>
+      </c>
+      <c r="B658" t="s">
+        <v>129</v>
+      </c>
+      <c r="C658" t="s">
+        <v>507</v>
+      </c>
+      <c r="D658" s="1">
+        <v>39</v>
+      </c>
+      <c r="L658" t="s">
+        <v>194</v>
+      </c>
+      <c r="M658" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="659" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A659">
+        <v>8</v>
+      </c>
+      <c r="B659" t="s">
+        <v>129</v>
+      </c>
+      <c r="C659" t="s">
+        <v>507</v>
+      </c>
+      <c r="D659" s="1">
+        <v>40</v>
+      </c>
+      <c r="L659" t="s">
+        <v>194</v>
+      </c>
+      <c r="M659" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="660" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A660">
+        <v>8</v>
+      </c>
+      <c r="B660" t="s">
+        <v>129</v>
+      </c>
+      <c r="C660" t="s">
+        <v>507</v>
+      </c>
+      <c r="D660" s="1">
+        <v>41</v>
+      </c>
+      <c r="L660" t="s">
+        <v>194</v>
+      </c>
+      <c r="M660" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="661" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A661">
+        <v>8</v>
+      </c>
+      <c r="B661" t="s">
+        <v>129</v>
+      </c>
+      <c r="C661" t="s">
+        <v>507</v>
+      </c>
+      <c r="D661" s="1">
+        <v>42</v>
+      </c>
+      <c r="L661" t="s">
+        <v>194</v>
+      </c>
+      <c r="M661" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="662" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A662">
+        <v>8</v>
+      </c>
+      <c r="B662" t="s">
+        <v>129</v>
+      </c>
+      <c r="C662" t="s">
+        <v>507</v>
+      </c>
+      <c r="D662" s="1">
+        <v>43</v>
+      </c>
+      <c r="L662" t="s">
+        <v>194</v>
+      </c>
+      <c r="M662" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="663" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A663">
+        <v>8</v>
+      </c>
+      <c r="B663" t="s">
+        <v>129</v>
+      </c>
+      <c r="C663" t="s">
+        <v>507</v>
+      </c>
+      <c r="D663" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="L663" t="s">
+        <v>69</v>
+      </c>
+      <c r="N663" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="664" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A664">
+        <v>8</v>
+      </c>
+      <c r="B664" t="s">
+        <v>129</v>
+      </c>
+      <c r="C664" t="s">
+        <v>507</v>
+      </c>
+      <c r="D664" s="1">
+        <v>45</v>
+      </c>
+      <c r="L664" t="s">
+        <v>46</v>
+      </c>
+      <c r="M664" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="665" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A665">
+        <v>8</v>
+      </c>
+      <c r="B665" t="s">
+        <v>129</v>
+      </c>
+      <c r="C665" t="s">
+        <v>507</v>
+      </c>
+      <c r="D665" s="1">
+        <v>46</v>
+      </c>
+      <c r="L665" t="s">
+        <v>194</v>
+      </c>
+      <c r="M665" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="666" spans="1:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="A666">
+        <v>8</v>
+      </c>
+      <c r="B666" t="s">
+        <v>129</v>
+      </c>
+      <c r="C666" t="s">
+        <v>507</v>
+      </c>
+      <c r="D666" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="L666" t="s">
+        <v>69</v>
+      </c>
+      <c r="N666" t="s">
+        <v>46</v>
+      </c>
+      <c r="O666" t="s">
+        <v>69</v>
+      </c>
+      <c r="P666" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q666" t="s">
+        <v>533</v>
+      </c>
+      <c r="R666" t="s">
+        <v>534</v>
+      </c>
+      <c r="S666" t="s">
+        <v>500</v>
+      </c>
+      <c r="T666">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="667" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A667">
+        <v>8</v>
+      </c>
+      <c r="B667" t="s">
+        <v>129</v>
+      </c>
+      <c r="C667" t="s">
+        <v>507</v>
+      </c>
+      <c r="D667" s="1">
+        <v>48</v>
+      </c>
+      <c r="L667" t="s">
+        <v>46</v>
+      </c>
+      <c r="M667" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="668" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A668">
+        <v>8</v>
+      </c>
+      <c r="B668" t="s">
+        <v>129</v>
+      </c>
+      <c r="C668" t="s">
+        <v>507</v>
+      </c>
+      <c r="D668" s="1">
+        <v>49</v>
+      </c>
+      <c r="L668" t="s">
+        <v>194</v>
+      </c>
+      <c r="M668" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="669" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A669">
+        <v>8</v>
+      </c>
+      <c r="B669" t="s">
+        <v>129</v>
+      </c>
+      <c r="C669" t="s">
+        <v>507</v>
+      </c>
+      <c r="D669" s="1">
+        <v>50</v>
+      </c>
+      <c r="L669" t="s">
+        <v>194</v>
+      </c>
+      <c r="M669" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="670" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A670">
+        <v>8</v>
+      </c>
+      <c r="B670" t="s">
+        <v>129</v>
+      </c>
+      <c r="C670" t="s">
+        <v>507</v>
+      </c>
+      <c r="D670" s="1">
+        <v>51</v>
+      </c>
+      <c r="L670" t="s">
+        <v>46</v>
+      </c>
+      <c r="M670" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="671" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A671">
+        <v>8</v>
+      </c>
+      <c r="B671" t="s">
+        <v>129</v>
+      </c>
+      <c r="C671" t="s">
+        <v>507</v>
+      </c>
+      <c r="D671" s="1">
+        <v>52</v>
+      </c>
+      <c r="L671" t="s">
+        <v>46</v>
+      </c>
+      <c r="M671" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="672" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A672">
+        <v>8</v>
+      </c>
+      <c r="B672" t="s">
+        <v>129</v>
+      </c>
+      <c r="C672" t="s">
+        <v>507</v>
+      </c>
+      <c r="D672" s="1">
+        <v>53</v>
+      </c>
+      <c r="L672" t="s">
+        <v>194</v>
+      </c>
+      <c r="M672" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="673" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A673">
+        <v>8</v>
+      </c>
+      <c r="B673" t="s">
+        <v>129</v>
+      </c>
+      <c r="C673" t="s">
+        <v>507</v>
+      </c>
+      <c r="D673" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="L673" t="s">
+        <v>69</v>
+      </c>
+      <c r="N673" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="674" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A674">
+        <v>8</v>
+      </c>
+      <c r="B674" t="s">
+        <v>129</v>
+      </c>
+      <c r="C674" t="s">
+        <v>507</v>
+      </c>
+      <c r="D674" s="1">
+        <v>55</v>
+      </c>
+      <c r="L674" t="s">
+        <v>46</v>
+      </c>
+      <c r="M674" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="675" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A675">
+        <v>8</v>
+      </c>
+      <c r="B675" t="s">
+        <v>129</v>
+      </c>
+      <c r="C675" t="s">
+        <v>507</v>
+      </c>
+      <c r="D675" s="1">
+        <v>56</v>
+      </c>
+      <c r="L675" t="s">
+        <v>46</v>
+      </c>
+      <c r="M675" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="676" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A676">
+        <v>8</v>
+      </c>
+      <c r="B676" t="s">
+        <v>129</v>
+      </c>
+      <c r="C676" t="s">
+        <v>507</v>
+      </c>
+      <c r="D676" s="1">
+        <v>57</v>
+      </c>
+      <c r="L676" t="s">
+        <v>46</v>
+      </c>
+      <c r="M676" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="677" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A677">
+        <v>8</v>
+      </c>
+      <c r="B677" t="s">
+        <v>129</v>
+      </c>
+      <c r="C677" t="s">
+        <v>507</v>
+      </c>
+      <c r="D677" s="1">
+        <v>58</v>
+      </c>
+      <c r="L677" t="s">
+        <v>46</v>
+      </c>
+      <c r="M677" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="678" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A678">
+        <v>8</v>
+      </c>
+      <c r="B678" t="s">
+        <v>129</v>
+      </c>
+      <c r="C678" t="s">
+        <v>507</v>
+      </c>
+      <c r="D678" s="1">
+        <v>59</v>
+      </c>
+      <c r="L678" t="s">
+        <v>46</v>
+      </c>
+      <c r="M678" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="679" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A679">
+        <v>8</v>
+      </c>
+      <c r="B679" t="s">
+        <v>129</v>
+      </c>
+      <c r="C679" t="s">
+        <v>507</v>
+      </c>
+      <c r="D679" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="L679" t="s">
+        <v>69</v>
+      </c>
+      <c r="N679" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="680" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A680">
+        <v>8</v>
+      </c>
+      <c r="B680" t="s">
+        <v>129</v>
+      </c>
+      <c r="C680" t="s">
+        <v>507</v>
+      </c>
+      <c r="D680" s="1">
+        <v>61</v>
+      </c>
+      <c r="L680" t="s">
+        <v>46</v>
+      </c>
+      <c r="M680" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="681" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A681">
+        <v>8</v>
+      </c>
+      <c r="B681" t="s">
+        <v>129</v>
+      </c>
+      <c r="C681" t="s">
+        <v>507</v>
+      </c>
+      <c r="D681" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="L681" t="s">
+        <v>69</v>
+      </c>
+      <c r="N681" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="682" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A682">
+        <v>8</v>
+      </c>
+      <c r="B682" t="s">
+        <v>129</v>
+      </c>
+      <c r="C682" t="s">
+        <v>507</v>
+      </c>
+      <c r="D682" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="L682" t="s">
+        <v>450</v>
+      </c>
+      <c r="M682" t="s">
+        <v>458</v>
+      </c>
+      <c r="N682" t="s">
+        <v>46</v>
+      </c>
+      <c r="O682" t="s">
+        <v>69</v>
+      </c>
+      <c r="P682" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q682" t="s">
+        <v>540</v>
+      </c>
+      <c r="S682" t="s">
+        <v>541</v>
+      </c>
+      <c r="T682">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="683" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A683">
+        <v>8</v>
+      </c>
+      <c r="B683" t="s">
+        <v>129</v>
+      </c>
+      <c r="C683" t="s">
+        <v>507</v>
+      </c>
+      <c r="D683" s="1">
+        <v>64</v>
+      </c>
+      <c r="L683" t="s">
+        <v>63</v>
+      </c>
+      <c r="M683" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="684" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A684">
+        <v>8</v>
+      </c>
+      <c r="B684" t="s">
+        <v>129</v>
+      </c>
+      <c r="C684" t="s">
+        <v>507</v>
+      </c>
+      <c r="D684" s="1">
+        <v>65</v>
+      </c>
+      <c r="L684" t="s">
+        <v>194</v>
+      </c>
+      <c r="M684" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="685" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A685">
+        <v>8</v>
+      </c>
+      <c r="B685" t="s">
+        <v>129</v>
+      </c>
+      <c r="C685" t="s">
+        <v>507</v>
+      </c>
+      <c r="D685" s="1">
+        <v>66</v>
+      </c>
+      <c r="L685" t="s">
+        <v>194</v>
+      </c>
+      <c r="M685" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="686" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A686">
+        <v>8</v>
+      </c>
+      <c r="B686" t="s">
+        <v>129</v>
+      </c>
+      <c r="C686" t="s">
+        <v>507</v>
+      </c>
+      <c r="D686" s="1">
+        <v>67</v>
+      </c>
+      <c r="L686" t="s">
+        <v>194</v>
+      </c>
+      <c r="M686" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="687" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A687">
+        <v>8</v>
+      </c>
+      <c r="B687" t="s">
+        <v>129</v>
+      </c>
+      <c r="C687" t="s">
+        <v>507</v>
+      </c>
+      <c r="D687" s="1">
+        <v>68</v>
+      </c>
+      <c r="L687" t="s">
+        <v>194</v>
+      </c>
+      <c r="M687" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="688" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A688">
+        <v>8</v>
+      </c>
+      <c r="B688" t="s">
+        <v>129</v>
+      </c>
+      <c r="C688" t="s">
+        <v>507</v>
+      </c>
+      <c r="D688" s="1">
+        <v>69</v>
+      </c>
+      <c r="L688" t="s">
+        <v>194</v>
+      </c>
+      <c r="M688" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="689" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A689">
+        <v>8</v>
+      </c>
+      <c r="B689" t="s">
+        <v>129</v>
+      </c>
+      <c r="C689" t="s">
+        <v>507</v>
+      </c>
+      <c r="D689" s="1">
+        <v>70</v>
+      </c>
+      <c r="L689" t="s">
+        <v>194</v>
+      </c>
+      <c r="M689" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="690" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A690">
+        <v>8</v>
+      </c>
+      <c r="B690" t="s">
+        <v>129</v>
+      </c>
+      <c r="C690" t="s">
+        <v>507</v>
+      </c>
+      <c r="D690" s="1">
+        <v>71</v>
+      </c>
+      <c r="L690" t="s">
+        <v>194</v>
+      </c>
+      <c r="M690" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="691" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A691">
+        <v>8</v>
+      </c>
+      <c r="B691" t="s">
+        <v>129</v>
+      </c>
+      <c r="C691" t="s">
+        <v>507</v>
+      </c>
+      <c r="D691" s="1">
+        <v>72</v>
+      </c>
+      <c r="L691" t="s">
+        <v>194</v>
+      </c>
+      <c r="M691" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="692" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A692">
+        <v>8</v>
+      </c>
+      <c r="B692" t="s">
+        <v>129</v>
+      </c>
+      <c r="C692" t="s">
+        <v>507</v>
+      </c>
+      <c r="D692" s="1">
+        <v>73</v>
+      </c>
+      <c r="L692" t="s">
+        <v>194</v>
+      </c>
+      <c r="M692" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="693" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A693">
+        <v>8</v>
+      </c>
+      <c r="B693" t="s">
+        <v>129</v>
+      </c>
+      <c r="C693" t="s">
+        <v>507</v>
+      </c>
+      <c r="D693" s="1">
+        <v>74</v>
+      </c>
+      <c r="L693" t="s">
+        <v>194</v>
+      </c>
+      <c r="M693" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="694" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A694">
+        <v>8</v>
+      </c>
+      <c r="B694" t="s">
+        <v>129</v>
+      </c>
+      <c r="C694" t="s">
+        <v>507</v>
+      </c>
+      <c r="D694" s="1">
+        <v>75</v>
+      </c>
+      <c r="L694" t="s">
+        <v>194</v>
+      </c>
+      <c r="M694" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="695" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A695">
+        <v>8</v>
+      </c>
+      <c r="B695" t="s">
+        <v>129</v>
+      </c>
+      <c r="C695" t="s">
+        <v>507</v>
+      </c>
+      <c r="D695" s="1">
+        <v>76</v>
+      </c>
+      <c r="L695" t="s">
+        <v>194</v>
+      </c>
+      <c r="M695" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="696" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A696">
+        <v>8</v>
+      </c>
+      <c r="B696" t="s">
+        <v>129</v>
+      </c>
+      <c r="C696" t="s">
+        <v>507</v>
+      </c>
+      <c r="D696" s="1">
+        <v>77</v>
+      </c>
+      <c r="L696" t="s">
+        <v>194</v>
+      </c>
+      <c r="M696" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="697" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A697">
+        <v>8</v>
+      </c>
+      <c r="B697" t="s">
+        <v>129</v>
+      </c>
+      <c r="C697" t="s">
+        <v>507</v>
+      </c>
+      <c r="D697" s="1">
+        <v>78</v>
+      </c>
+      <c r="L697" t="s">
+        <v>194</v>
+      </c>
+      <c r="M697" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="698" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A698">
+        <v>8</v>
+      </c>
+      <c r="B698" t="s">
+        <v>129</v>
+      </c>
+      <c r="C698" t="s">
+        <v>507</v>
+      </c>
+      <c r="D698" s="1">
+        <v>79</v>
+      </c>
+      <c r="L698" t="s">
+        <v>194</v>
+      </c>
+      <c r="M698" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="699" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A699">
+        <v>8</v>
+      </c>
+      <c r="B699" t="s">
+        <v>129</v>
+      </c>
+      <c r="C699" t="s">
+        <v>507</v>
+      </c>
+      <c r="D699" s="1">
+        <v>80</v>
+      </c>
+      <c r="L699" t="s">
+        <v>194</v>
+      </c>
+      <c r="M699" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="700" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A700">
+        <v>8</v>
+      </c>
+      <c r="B700" t="s">
+        <v>129</v>
+      </c>
+      <c r="C700" t="s">
+        <v>507</v>
+      </c>
+      <c r="D700" s="1">
+        <v>81</v>
+      </c>
+      <c r="L700" t="s">
+        <v>194</v>
+      </c>
+      <c r="M700" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="701" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A701">
+        <v>8</v>
+      </c>
+      <c r="B701" t="s">
+        <v>129</v>
+      </c>
+      <c r="C701" t="s">
+        <v>507</v>
+      </c>
+      <c r="D701" s="1">
+        <v>82</v>
+      </c>
+      <c r="L701" t="s">
+        <v>194</v>
+      </c>
+      <c r="M701" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="702" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A702">
+        <v>8</v>
+      </c>
+      <c r="B702" t="s">
+        <v>129</v>
+      </c>
+      <c r="C702" t="s">
+        <v>507</v>
+      </c>
+      <c r="D702" s="1">
+        <v>83</v>
+      </c>
+      <c r="L702" t="s">
+        <v>194</v>
+      </c>
+      <c r="M702" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="703" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A703">
+        <v>8</v>
+      </c>
+      <c r="B703" t="s">
+        <v>129</v>
+      </c>
+      <c r="C703" t="s">
+        <v>507</v>
+      </c>
+      <c r="D703" s="1">
+        <v>84</v>
+      </c>
+      <c r="L703" t="s">
+        <v>194</v>
+      </c>
+      <c r="M703" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="704" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A704">
+        <v>8</v>
+      </c>
+      <c r="B704" t="s">
+        <v>129</v>
+      </c>
+      <c r="C704" t="s">
+        <v>507</v>
+      </c>
+      <c r="D704" s="1">
+        <v>85</v>
+      </c>
+      <c r="L704" t="s">
+        <v>194</v>
+      </c>
+      <c r="M704" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="705" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A705">
+        <v>8</v>
+      </c>
+      <c r="B705" t="s">
+        <v>129</v>
+      </c>
+      <c r="C705" t="s">
+        <v>507</v>
+      </c>
+      <c r="D705" s="1">
+        <v>86</v>
+      </c>
+      <c r="L705" t="s">
+        <v>194</v>
+      </c>
+      <c r="M705" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="706" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A706">
+        <v>8</v>
+      </c>
+      <c r="B706" t="s">
+        <v>129</v>
+      </c>
+      <c r="C706" t="s">
+        <v>507</v>
+      </c>
+      <c r="D706" s="1">
+        <v>87</v>
+      </c>
+      <c r="L706" t="s">
+        <v>194</v>
+      </c>
+      <c r="M706" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="707" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A707">
+        <v>8</v>
+      </c>
+      <c r="B707" t="s">
+        <v>129</v>
+      </c>
+      <c r="C707" t="s">
+        <v>507</v>
+      </c>
+      <c r="D707" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="L707" t="s">
+        <v>69</v>
+      </c>
+      <c r="N707" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="708" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A708">
+        <v>8</v>
+      </c>
+      <c r="B708" t="s">
+        <v>129</v>
+      </c>
+      <c r="C708" t="s">
+        <v>507</v>
+      </c>
+      <c r="D708" s="1">
+        <v>89</v>
+      </c>
+      <c r="L708" t="s">
+        <v>194</v>
+      </c>
+      <c r="M708" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="709" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A709">
+        <v>8</v>
+      </c>
+      <c r="B709" t="s">
+        <v>129</v>
+      </c>
+      <c r="C709" t="s">
+        <v>507</v>
+      </c>
+      <c r="D709" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="L709" t="s">
+        <v>69</v>
+      </c>
+      <c r="N709" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="710" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A710">
+        <v>8</v>
+      </c>
+      <c r="B710" t="s">
+        <v>129</v>
+      </c>
+      <c r="C710" t="s">
+        <v>507</v>
+      </c>
+      <c r="D710" s="1">
+        <v>91</v>
+      </c>
+      <c r="L710" t="s">
+        <v>46</v>
+      </c>
+      <c r="M710" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="711" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A711">
+        <v>8</v>
+      </c>
+      <c r="B711" t="s">
+        <v>129</v>
+      </c>
+      <c r="C711" t="s">
+        <v>507</v>
+      </c>
+      <c r="D711" s="1">
+        <v>92</v>
+      </c>
+      <c r="L711" t="s">
+        <v>194</v>
+      </c>
+      <c r="M711" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="712" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A712">
+        <v>8</v>
+      </c>
+      <c r="B712" t="s">
+        <v>129</v>
+      </c>
+      <c r="C712" t="s">
+        <v>507</v>
+      </c>
+      <c r="D712" s="1">
+        <v>93</v>
+      </c>
+      <c r="L712" t="s">
+        <v>194</v>
+      </c>
+      <c r="M712" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="713" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A713">
+        <v>8</v>
+      </c>
+      <c r="B713" t="s">
+        <v>129</v>
+      </c>
+      <c r="C713" t="s">
+        <v>507</v>
+      </c>
+      <c r="D713" s="1">
+        <v>94</v>
+      </c>
+      <c r="L713" t="s">
+        <v>194</v>
+      </c>
+      <c r="M713" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="714" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A714">
+        <v>8</v>
+      </c>
+      <c r="B714" t="s">
+        <v>129</v>
+      </c>
+      <c r="C714" t="s">
+        <v>507</v>
+      </c>
+      <c r="D714" s="1">
+        <v>95</v>
+      </c>
+      <c r="L714" t="s">
+        <v>194</v>
+      </c>
+      <c r="M714" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="715" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A715">
+        <v>8</v>
+      </c>
+      <c r="B715" t="s">
+        <v>129</v>
+      </c>
+      <c r="C715" t="s">
+        <v>507</v>
+      </c>
+      <c r="D715" s="1">
+        <v>96</v>
+      </c>
+      <c r="L715" t="s">
+        <v>194</v>
+      </c>
+      <c r="M715" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="716" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A716">
+        <v>8</v>
+      </c>
+      <c r="B716" t="s">
+        <v>129</v>
+      </c>
+      <c r="C716" t="s">
+        <v>507</v>
+      </c>
+      <c r="D716" s="1">
+        <v>97</v>
+      </c>
+      <c r="L716" t="s">
+        <v>194</v>
+      </c>
+      <c r="M716" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="717" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A717">
+        <v>9</v>
+      </c>
+      <c r="B717" t="s">
+        <v>129</v>
+      </c>
+      <c r="C717" t="s">
+        <v>507</v>
+      </c>
+      <c r="D717" s="1">
+        <v>1</v>
+      </c>
+      <c r="L717" t="s">
+        <v>194</v>
+      </c>
+      <c r="M717" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="718" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A718">
+        <v>9</v>
+      </c>
+      <c r="B718" t="s">
+        <v>129</v>
+      </c>
+      <c r="C718" t="s">
+        <v>507</v>
+      </c>
+      <c r="D718" s="1">
+        <v>2</v>
+      </c>
+      <c r="L718" t="s">
+        <v>194</v>
+      </c>
+      <c r="M718" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="719" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A719">
+        <v>9</v>
+      </c>
+      <c r="B719" t="s">
+        <v>129</v>
+      </c>
+      <c r="C719" t="s">
+        <v>507</v>
+      </c>
+      <c r="D719" s="1">
+        <v>3</v>
+      </c>
+      <c r="L719" t="s">
+        <v>194</v>
+      </c>
+      <c r="M719" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="720" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A720">
+        <v>9</v>
+      </c>
+      <c r="B720" t="s">
+        <v>129</v>
+      </c>
+      <c r="C720" t="s">
+        <v>507</v>
+      </c>
+      <c r="D720" s="1">
+        <v>4</v>
+      </c>
+      <c r="L720" t="s">
+        <v>194</v>
+      </c>
+      <c r="M720" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="721" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A721">
+        <v>9</v>
+      </c>
+      <c r="B721" t="s">
+        <v>129</v>
+      </c>
+      <c r="C721" t="s">
+        <v>507</v>
+      </c>
+      <c r="D721" s="1">
+        <v>5</v>
+      </c>
+      <c r="L721" t="s">
+        <v>194</v>
+      </c>
+      <c r="M721" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="722" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A722">
+        <v>9</v>
+      </c>
+      <c r="B722" t="s">
+        <v>129</v>
+      </c>
+      <c r="C722" t="s">
+        <v>507</v>
+      </c>
+      <c r="D722" s="1">
+        <v>6</v>
+      </c>
+      <c r="L722" t="s">
+        <v>194</v>
+      </c>
+      <c r="M722" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="723" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A723">
+        <v>9</v>
+      </c>
+      <c r="B723" t="s">
+        <v>129</v>
+      </c>
+      <c r="C723" t="s">
+        <v>507</v>
+      </c>
+      <c r="D723" s="1">
+        <v>7</v>
+      </c>
+      <c r="L723" t="s">
+        <v>194</v>
+      </c>
+      <c r="M723" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="724" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A724">
+        <v>9</v>
+      </c>
+      <c r="B724" t="s">
+        <v>129</v>
+      </c>
+      <c r="C724" t="s">
+        <v>507</v>
+      </c>
+      <c r="D724" s="1">
+        <v>8</v>
+      </c>
+      <c r="L724" t="s">
+        <v>194</v>
+      </c>
+      <c r="M724" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="725" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A725">
+        <v>9</v>
+      </c>
+      <c r="B725" t="s">
+        <v>129</v>
+      </c>
+      <c r="C725" t="s">
+        <v>507</v>
+      </c>
+      <c r="D725" s="1">
+        <v>9</v>
+      </c>
+      <c r="L725" t="s">
+        <v>194</v>
+      </c>
+      <c r="M725" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="726" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A726">
+        <v>9</v>
+      </c>
+      <c r="B726" t="s">
+        <v>129</v>
+      </c>
+      <c r="C726" t="s">
+        <v>507</v>
+      </c>
+      <c r="D726" s="1">
+        <v>10</v>
+      </c>
+      <c r="L726" t="s">
+        <v>194</v>
+      </c>
+      <c r="M726" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="727" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A727">
+        <v>9</v>
+      </c>
+      <c r="B727" t="s">
+        <v>129</v>
+      </c>
+      <c r="C727" t="s">
+        <v>507</v>
+      </c>
+      <c r="D727" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="L727" t="s">
+        <v>69</v>
+      </c>
+      <c r="M727" t="s">
+        <v>458</v>
+      </c>
+      <c r="N727" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="728" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A728">
+        <v>9</v>
+      </c>
+      <c r="B728" t="s">
+        <v>129</v>
+      </c>
+      <c r="C728" t="s">
+        <v>507</v>
+      </c>
+      <c r="D728" s="1">
+        <v>112</v>
+      </c>
+      <c r="L728" t="s">
+        <v>194</v>
+      </c>
+      <c r="M728" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="729" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A729">
+        <v>9</v>
+      </c>
+      <c r="B729" t="s">
+        <v>129</v>
+      </c>
+      <c r="C729" t="s">
+        <v>507</v>
+      </c>
+      <c r="D729" s="1">
+        <v>113</v>
+      </c>
+      <c r="L729" t="s">
+        <v>194</v>
+      </c>
+      <c r="M729" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="730" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A730">
+        <v>9</v>
+      </c>
+      <c r="B730" t="s">
+        <v>129</v>
+      </c>
+      <c r="C730" t="s">
+        <v>507</v>
+      </c>
+      <c r="D730" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="L730" t="s">
+        <v>69</v>
+      </c>
+      <c r="N730" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="731" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A731">
+        <v>9</v>
+      </c>
+      <c r="B731" t="s">
+        <v>129</v>
+      </c>
+      <c r="C731" t="s">
+        <v>507</v>
+      </c>
+      <c r="D731" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="L731" t="s">
+        <v>69</v>
+      </c>
+      <c r="N731" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="732" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A732">
+        <v>9</v>
+      </c>
+      <c r="B732" t="s">
+        <v>129</v>
+      </c>
+      <c r="C732" t="s">
+        <v>507</v>
+      </c>
+      <c r="D732" s="1">
+        <v>116</v>
+      </c>
+      <c r="L732" t="s">
+        <v>194</v>
+      </c>
+      <c r="M732" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="733" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A733">
+        <v>9</v>
+      </c>
+      <c r="B733" t="s">
+        <v>129</v>
+      </c>
+      <c r="C733" t="s">
+        <v>507</v>
+      </c>
+      <c r="D733" s="1">
+        <v>117</v>
+      </c>
+      <c r="L733" t="s">
+        <v>194</v>
+      </c>
+      <c r="M733" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="734" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A734">
+        <v>9</v>
+      </c>
+      <c r="B734" t="s">
+        <v>129</v>
+      </c>
+      <c r="C734" t="s">
+        <v>507</v>
+      </c>
+      <c r="D734" s="1">
+        <v>118</v>
+      </c>
+      <c r="L734" t="s">
+        <v>194</v>
+      </c>
+      <c r="M734" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="735" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A735">
+        <v>9</v>
+      </c>
+      <c r="B735" t="s">
+        <v>129</v>
+      </c>
+      <c r="C735" t="s">
+        <v>507</v>
+      </c>
+      <c r="D735" s="1">
+        <v>119</v>
+      </c>
+      <c r="L735" t="s">
+        <v>194</v>
+      </c>
+      <c r="M735" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="736" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A736">
+        <v>9</v>
+      </c>
+      <c r="B736" t="s">
+        <v>129</v>
+      </c>
+      <c r="C736" t="s">
+        <v>507</v>
+      </c>
+      <c r="D736" s="1">
+        <v>120</v>
+      </c>
+      <c r="L736" t="s">
+        <v>194</v>
+      </c>
+      <c r="M736" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="737" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A737">
+        <v>9</v>
+      </c>
+      <c r="B737" t="s">
+        <v>129</v>
+      </c>
+      <c r="C737" t="s">
+        <v>507</v>
+      </c>
+      <c r="D737" s="1">
+        <v>121</v>
+      </c>
+      <c r="L737" t="s">
+        <v>194</v>
+      </c>
+      <c r="M737" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="738" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A738">
+        <v>9</v>
+      </c>
+      <c r="B738" t="s">
+        <v>129</v>
+      </c>
+      <c r="C738" t="s">
+        <v>507</v>
+      </c>
+      <c r="D738" s="1">
+        <v>122</v>
+      </c>
+      <c r="L738" t="s">
+        <v>194</v>
+      </c>
+      <c r="M738" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="739" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A739">
+        <v>9</v>
+      </c>
+      <c r="B739" t="s">
+        <v>129</v>
+      </c>
+      <c r="C739" t="s">
+        <v>507</v>
+      </c>
+      <c r="D739" s="1">
+        <v>123</v>
+      </c>
+      <c r="L739" t="s">
+        <v>194</v>
+      </c>
+      <c r="M739" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="740" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A740">
+        <v>9</v>
+      </c>
+      <c r="B740" t="s">
+        <v>129</v>
+      </c>
+      <c r="C740" t="s">
+        <v>507</v>
+      </c>
+      <c r="D740" s="1">
+        <v>124</v>
+      </c>
+      <c r="L740" t="s">
+        <v>194</v>
+      </c>
+      <c r="M740" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="741" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A741">
+        <v>9</v>
+      </c>
+      <c r="B741" t="s">
+        <v>129</v>
+      </c>
+      <c r="C741" t="s">
+        <v>507</v>
+      </c>
+      <c r="D741" s="1">
+        <v>125</v>
+      </c>
+      <c r="L741" t="s">
+        <v>194</v>
+      </c>
+      <c r="M741" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="742" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A742">
+        <v>9</v>
+      </c>
+      <c r="B742" t="s">
+        <v>129</v>
+      </c>
+      <c r="C742" t="s">
+        <v>507</v>
+      </c>
+      <c r="D742" s="1">
+        <v>126</v>
+      </c>
+      <c r="L742" t="s">
+        <v>194</v>
+      </c>
+      <c r="M742" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="743" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A743">
+        <v>9</v>
+      </c>
+      <c r="B743" t="s">
+        <v>129</v>
+      </c>
+      <c r="C743" t="s">
+        <v>507</v>
+      </c>
+      <c r="D743" s="1">
+        <v>127</v>
+      </c>
+      <c r="L743" t="s">
+        <v>194</v>
+      </c>
+      <c r="M743" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="744" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A744">
+        <v>9</v>
+      </c>
+      <c r="B744" t="s">
+        <v>129</v>
+      </c>
+      <c r="C744" t="s">
+        <v>507</v>
+      </c>
+      <c r="D744" s="1">
+        <v>128</v>
+      </c>
+      <c r="L744" t="s">
+        <v>194</v>
+      </c>
+      <c r="M744" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="745" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A745">
+        <v>9</v>
+      </c>
+      <c r="B745" t="s">
+        <v>129</v>
+      </c>
+      <c r="C745" t="s">
+        <v>507</v>
+      </c>
+      <c r="D745" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="L745" t="s">
+        <v>69</v>
+      </c>
+      <c r="N745" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="746" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A746">
+        <v>9</v>
+      </c>
+      <c r="B746" t="s">
+        <v>129</v>
+      </c>
+      <c r="C746" t="s">
+        <v>507</v>
+      </c>
+      <c r="D746" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="L746" t="s">
+        <v>69</v>
+      </c>
+      <c r="N746" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="747" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A747">
+        <v>9</v>
+      </c>
+      <c r="B747" t="s">
+        <v>129</v>
+      </c>
+      <c r="C747" t="s">
+        <v>507</v>
+      </c>
+      <c r="D747" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="L747" t="s">
+        <v>69</v>
+      </c>
+      <c r="N747" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="748" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A748">
+        <v>9</v>
+      </c>
+      <c r="B748" t="s">
+        <v>129</v>
+      </c>
+      <c r="C748" t="s">
+        <v>507</v>
+      </c>
+      <c r="D748" s="1">
+        <v>132</v>
+      </c>
+      <c r="L748" t="s">
+        <v>194</v>
+      </c>
+      <c r="M748" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="749" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A749">
+        <v>9</v>
+      </c>
+      <c r="B749" t="s">
+        <v>129</v>
+      </c>
+      <c r="C749" t="s">
+        <v>507</v>
+      </c>
+      <c r="D749" s="1">
+        <v>133</v>
+      </c>
+      <c r="L749" t="s">
+        <v>194</v>
+      </c>
+      <c r="M749" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="750" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A750">
+        <v>9</v>
+      </c>
+      <c r="B750" t="s">
+        <v>129</v>
+      </c>
+      <c r="C750" t="s">
+        <v>507</v>
+      </c>
+      <c r="D750" s="1">
+        <v>134</v>
+      </c>
+      <c r="L750" t="s">
+        <v>194</v>
+      </c>
+      <c r="M750" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="751" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A751">
+        <v>9</v>
+      </c>
+      <c r="B751" t="s">
+        <v>129</v>
+      </c>
+      <c r="C751" t="s">
+        <v>507</v>
+      </c>
+      <c r="D751" s="1">
+        <v>135</v>
+      </c>
+      <c r="L751" t="s">
+        <v>194</v>
+      </c>
+      <c r="M751" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="752" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A752">
+        <v>9</v>
+      </c>
+      <c r="B752" t="s">
+        <v>129</v>
+      </c>
+      <c r="C752" t="s">
+        <v>507</v>
+      </c>
+      <c r="D752" s="1">
+        <v>136</v>
+      </c>
+      <c r="L752" t="s">
+        <v>194</v>
+      </c>
+      <c r="M752" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="753" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A753">
+        <v>9</v>
+      </c>
+      <c r="B753" t="s">
+        <v>129</v>
+      </c>
+      <c r="C753" t="s">
+        <v>507</v>
+      </c>
+      <c r="D753" s="1">
+        <v>137</v>
+      </c>
+      <c r="L753" t="s">
+        <v>194</v>
+      </c>
+      <c r="M753" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="754" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A754">
+        <v>9</v>
+      </c>
+      <c r="B754" t="s">
+        <v>129</v>
+      </c>
+      <c r="C754" t="s">
+        <v>507</v>
+      </c>
+      <c r="D754" s="1">
+        <v>138</v>
+      </c>
+      <c r="L754" t="s">
+        <v>194</v>
+      </c>
+      <c r="M754" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="755" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A755">
+        <v>9</v>
+      </c>
+      <c r="B755" t="s">
+        <v>129</v>
+      </c>
+      <c r="C755" t="s">
+        <v>507</v>
+      </c>
+      <c r="D755" s="1">
+        <v>139</v>
+      </c>
+      <c r="L755" t="s">
+        <v>194</v>
+      </c>
+      <c r="M755" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="756" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A756">
+        <v>9</v>
+      </c>
+      <c r="B756" t="s">
+        <v>129</v>
+      </c>
+      <c r="C756" t="s">
+        <v>507</v>
+      </c>
+      <c r="D756" s="1">
+        <v>140</v>
+      </c>
+      <c r="L756" t="s">
+        <v>194</v>
+      </c>
+      <c r="M756" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="757" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A757">
+        <v>9</v>
+      </c>
+      <c r="B757" t="s">
+        <v>129</v>
+      </c>
+      <c r="C757" t="s">
+        <v>507</v>
+      </c>
+      <c r="D757" s="1">
+        <v>141</v>
+      </c>
+      <c r="L757" t="s">
+        <v>194</v>
+      </c>
+      <c r="M757" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="758" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A758">
+        <v>9</v>
+      </c>
+      <c r="B758" t="s">
+        <v>129</v>
+      </c>
+      <c r="C758" t="s">
+        <v>507</v>
+      </c>
+      <c r="D758" s="1">
+        <v>142</v>
+      </c>
+      <c r="L758" t="s">
+        <v>450</v>
+      </c>
+      <c r="M758" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="759" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A759">
+        <v>9</v>
+      </c>
+      <c r="B759" t="s">
+        <v>129</v>
+      </c>
+      <c r="C759" t="s">
+        <v>507</v>
+      </c>
+      <c r="D759" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="L759" t="s">
+        <v>69</v>
+      </c>
+      <c r="N759" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="760" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A760">
+        <v>9</v>
+      </c>
+      <c r="B760" t="s">
+        <v>129</v>
+      </c>
+      <c r="C760" t="s">
+        <v>507</v>
+      </c>
+      <c r="D760" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="L760" t="s">
+        <v>227</v>
+      </c>
+      <c r="N760" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="761" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A761">
+        <v>9</v>
+      </c>
+      <c r="B761" t="s">
+        <v>129</v>
+      </c>
+      <c r="C761" t="s">
+        <v>507</v>
+      </c>
+      <c r="D761" s="1">
+        <v>145</v>
+      </c>
+      <c r="L761" t="s">
+        <v>194</v>
+      </c>
+      <c r="M761" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="762" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A762">
+        <v>10</v>
+      </c>
+      <c r="B762" t="s">
+        <v>129</v>
+      </c>
+      <c r="D762" s="1">
+        <v>146</v>
+      </c>
+      <c r="L762" t="s">
+        <v>194</v>
+      </c>
+      <c r="M762" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="763" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A763">
+        <v>10</v>
+      </c>
+      <c r="B763" t="s">
+        <v>129</v>
+      </c>
+      <c r="D763" s="1">
+        <v>147</v>
+      </c>
+      <c r="L763" t="s">
+        <v>194</v>
+      </c>
+      <c r="M763" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="764" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B764" t="s">
+        <v>129</v>
+      </c>
+      <c r="D764" s="1">
+        <v>1</v>
+      </c>
+      <c r="L764" t="s">
+        <v>194</v>
+      </c>
+      <c r="M764" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="765" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="B765" t="s">
+        <v>129</v>
+      </c>
+      <c r="D765" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="L765" t="s">
+        <v>69</v>
+      </c>
+      <c r="N765" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="766" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B766" t="s">
+        <v>129</v>
+      </c>
+      <c r="D766" s="1">
+        <v>3</v>
+      </c>
+      <c r="L766" t="s">
+        <v>194</v>
+      </c>
+      <c r="M766" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="767" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B767" t="s">
+        <v>129</v>
+      </c>
+      <c r="D767" s="1">
+        <v>4</v>
+      </c>
+      <c r="L767" t="s">
+        <v>194</v>
+      </c>
+      <c r="M767" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="768" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B768" t="s">
+        <v>129</v>
+      </c>
+      <c r="D768" s="1">
+        <v>5</v>
+      </c>
+      <c r="L768" t="s">
+        <v>194</v>
+      </c>
+      <c r="M768" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="769" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B769" t="s">
+        <v>129</v>
+      </c>
+      <c r="D769" s="1">
+        <v>6</v>
+      </c>
+      <c r="L769" t="s">
+        <v>194</v>
+      </c>
+      <c r="M769" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="770" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B770" t="s">
+        <v>129</v>
+      </c>
+      <c r="D770" s="1">
+        <v>7</v>
+      </c>
+      <c r="L770" t="s">
+        <v>194</v>
+      </c>
+      <c r="M770" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="771" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B771" t="s">
+        <v>129</v>
+      </c>
+      <c r="D771" s="1">
+        <v>8</v>
+      </c>
+      <c r="L771" t="s">
+        <v>194</v>
+      </c>
+      <c r="M771" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="772" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B772" t="s">
+        <v>129</v>
+      </c>
+      <c r="D772" s="1">
+        <v>9</v>
+      </c>
+      <c r="L772" t="s">
+        <v>194</v>
+      </c>
+      <c r="M772" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="773" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B773" t="s">
+        <v>129</v>
+      </c>
+      <c r="D773" s="1">
+        <v>10</v>
+      </c>
+      <c r="L773" t="s">
+        <v>194</v>
+      </c>
+      <c r="M773" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="774" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B774" t="s">
+        <v>129</v>
+      </c>
+      <c r="D774" s="1">
+        <v>11</v>
+      </c>
+      <c r="L774" t="s">
+        <v>194</v>
+      </c>
+      <c r="M774" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="775" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B775" t="s">
+        <v>129</v>
+      </c>
+      <c r="D775" s="1">
+        <v>12</v>
+      </c>
+      <c r="L775" t="s">
+        <v>194</v>
+      </c>
+      <c r="M775" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="776" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B776" t="s">
+        <v>129</v>
+      </c>
+      <c r="D776" s="1">
+        <v>13</v>
+      </c>
+      <c r="L776" t="s">
+        <v>194</v>
+      </c>
+      <c r="M776" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="777" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B777" t="s">
+        <v>129</v>
+      </c>
+      <c r="D777" s="1">
+        <v>14</v>
+      </c>
+      <c r="L777" t="s">
+        <v>194</v>
+      </c>
+      <c r="M777" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="778" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B778" t="s">
+        <v>129</v>
+      </c>
+      <c r="D778" s="1">
+        <v>15</v>
+      </c>
+      <c r="L778" t="s">
+        <v>194</v>
+      </c>
+      <c r="M778" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="779" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B779" t="s">
+        <v>129</v>
+      </c>
+      <c r="D779" s="1">
+        <v>16</v>
+      </c>
+      <c r="L779" t="s">
+        <v>194</v>
+      </c>
+      <c r="M779" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="780" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B780" t="s">
+        <v>129</v>
+      </c>
+      <c r="D780" s="1">
+        <v>17</v>
+      </c>
+      <c r="L780" t="s">
+        <v>194</v>
+      </c>
+      <c r="M780" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="781" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B781" t="s">
+        <v>129</v>
+      </c>
+      <c r="D781" s="1">
+        <v>18</v>
+      </c>
+      <c r="L781" t="s">
+        <v>194</v>
+      </c>
+      <c r="M781" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="782" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B782" t="s">
+        <v>129</v>
+      </c>
+      <c r="D782" s="1">
+        <v>19</v>
+      </c>
+      <c r="L782" t="s">
+        <v>194</v>
+      </c>
+      <c r="M782" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="783" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B783" t="s">
+        <v>129</v>
+      </c>
+      <c r="D783" s="1">
+        <v>20</v>
+      </c>
+      <c r="L783" t="s">
+        <v>194</v>
+      </c>
+      <c r="M783" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="784" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B784" t="s">
+        <v>129</v>
+      </c>
+      <c r="D784" s="1">
+        <v>21</v>
+      </c>
+      <c r="L784" t="s">
+        <v>194</v>
+      </c>
+      <c r="M784" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="785" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B785" t="s">
+        <v>129</v>
+      </c>
+      <c r="D785" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="L785" t="s">
+        <v>69</v>
+      </c>
+      <c r="N785" t="s">
+        <v>194</v>
+      </c>
+      <c r="O785" t="s">
+        <v>227</v>
+      </c>
+      <c r="P785" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q785" t="s">
+        <v>566</v>
+      </c>
+      <c r="R785" t="s">
+        <v>567</v>
+      </c>
+      <c r="S785" t="s">
+        <v>257</v>
+      </c>
+      <c r="T785">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="786" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B786" t="s">
+        <v>129</v>
+      </c>
+      <c r="D786" s="1">
+        <v>23</v>
+      </c>
+      <c r="L786" t="s">
+        <v>194</v>
+      </c>
+      <c r="M786" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="787" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B787" t="s">
+        <v>129</v>
+      </c>
+      <c r="D787" s="1">
+        <v>24</v>
+      </c>
+      <c r="L787" t="s">
+        <v>194</v>
+      </c>
+      <c r="M787" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="788" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B788" t="s">
+        <v>129</v>
+      </c>
+      <c r="D788" s="1">
+        <v>25</v>
+      </c>
+      <c r="L788" t="s">
+        <v>194</v>
+      </c>
+      <c r="M788" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="789" spans="2:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="B789" t="s">
+        <v>129</v>
+      </c>
+      <c r="D789" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="L789" t="s">
+        <v>69</v>
+      </c>
+      <c r="N789" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="790" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B790" t="s">
+        <v>129</v>
+      </c>
+      <c r="D790" s="1">
+        <v>27</v>
+      </c>
+      <c r="L790" t="s">
+        <v>194</v>
+      </c>
+      <c r="M790" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="791" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B791" t="s">
+        <v>129</v>
+      </c>
+      <c r="D791" s="1">
+        <v>28</v>
+      </c>
+      <c r="L791" t="s">
+        <v>194</v>
+      </c>
+      <c r="M791" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="792" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B792" t="s">
+        <v>129</v>
+      </c>
+      <c r="D792" s="1">
+        <v>29</v>
+      </c>
+      <c r="L792" t="s">
+        <v>194</v>
+      </c>
+      <c r="M792" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="793" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B793" t="s">
+        <v>129</v>
+      </c>
+      <c r="D793" s="1">
+        <v>30</v>
+      </c>
+      <c r="L793" t="s">
+        <v>194</v>
+      </c>
+      <c r="M793" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="794" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B794" t="s">
+        <v>129</v>
+      </c>
+      <c r="D794" s="1">
+        <v>31</v>
+      </c>
+      <c r="L794" t="s">
+        <v>194</v>
+      </c>
+      <c r="M794" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="795" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B795" t="s">
+        <v>129</v>
+      </c>
+      <c r="D795" s="1">
+        <v>32</v>
+      </c>
+      <c r="L795" t="s">
+        <v>194</v>
+      </c>
+      <c r="M795" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="796" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B796" t="s">
+        <v>129</v>
+      </c>
+      <c r="D796" s="1">
+        <v>33</v>
+      </c>
+      <c r="L796" t="s">
+        <v>194</v>
+      </c>
+      <c r="M796" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="797" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B797" t="s">
+        <v>129</v>
+      </c>
+      <c r="D797" s="1">
+        <v>34</v>
+      </c>
+      <c r="L797" t="s">
+        <v>194</v>
+      </c>
+      <c r="M797" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="798" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B798" t="s">
+        <v>129</v>
+      </c>
+      <c r="D798" s="1">
+        <v>35</v>
+      </c>
+      <c r="L798" t="s">
+        <v>194</v>
+      </c>
+      <c r="M798" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="799" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B799" t="s">
+        <v>129</v>
+      </c>
+      <c r="D799" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="L799" t="s">
+        <v>227</v>
+      </c>
+      <c r="N799" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="800" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B800" t="s">
+        <v>129</v>
+      </c>
+      <c r="D800" s="1">
+        <v>37</v>
+      </c>
+      <c r="L800" t="s">
+        <v>194</v>
+      </c>
+      <c r="M800" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="801" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B801" t="s">
+        <v>129</v>
+      </c>
+      <c r="D801" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="L801" t="s">
+        <v>69</v>
+      </c>
+      <c r="N801" t="s">
+        <v>46</v>
+      </c>
+      <c r="O801" t="s">
+        <v>69</v>
+      </c>
+      <c r="P801" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q801" t="s">
+        <v>572</v>
+      </c>
+      <c r="R801" t="s">
+        <v>573</v>
+      </c>
+      <c r="S801" t="s">
+        <v>574</v>
+      </c>
+      <c r="T801">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="802" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B802" t="s">
+        <v>129</v>
+      </c>
+      <c r="D802" s="1">
+        <v>39</v>
+      </c>
+      <c r="L802" t="s">
+        <v>194</v>
+      </c>
+      <c r="M802" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="803" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B803" t="s">
+        <v>129</v>
+      </c>
+      <c r="D803" s="1">
+        <v>40</v>
+      </c>
+      <c r="L803" t="s">
+        <v>194</v>
+      </c>
+      <c r="M803" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="804" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B804" t="s">
+        <v>129</v>
+      </c>
+      <c r="D804" s="1">
+        <v>41</v>
+      </c>
+      <c r="L804" t="s">
+        <v>194</v>
+      </c>
+      <c r="M804" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="805" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B805" t="s">
+        <v>129</v>
+      </c>
+      <c r="D805" s="1">
+        <v>42</v>
+      </c>
+      <c r="L805" t="s">
+        <v>194</v>
+      </c>
+      <c r="M805" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="806" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B806" t="s">
+        <v>129</v>
+      </c>
+      <c r="D806" s="1">
+        <v>43</v>
+      </c>
+      <c r="L806" t="s">
+        <v>194</v>
+      </c>
+      <c r="M806" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="807" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B807" t="s">
+        <v>129</v>
+      </c>
+      <c r="D807" s="1">
+        <v>44</v>
+      </c>
+      <c r="L807" t="s">
+        <v>194</v>
+      </c>
+      <c r="M807" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="808" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B808" t="s">
+        <v>129</v>
+      </c>
+      <c r="D808" s="1">
+        <v>45</v>
+      </c>
+      <c r="L808" t="s">
+        <v>194</v>
+      </c>
+      <c r="M808" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="809" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B809" t="s">
+        <v>129</v>
+      </c>
+      <c r="D809" s="1">
+        <v>46</v>
+      </c>
+      <c r="L809" t="s">
+        <v>194</v>
+      </c>
+      <c r="M809" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="810" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B810" t="s">
+        <v>129</v>
+      </c>
+      <c r="D810" s="1">
+        <v>47</v>
+      </c>
+      <c r="L810" t="s">
+        <v>194</v>
+      </c>
+      <c r="M810" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="811" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B811" t="s">
+        <v>129</v>
+      </c>
+      <c r="D811" s="1">
+        <v>48</v>
+      </c>
+      <c r="L811" t="s">
+        <v>194</v>
+      </c>
+      <c r="M811" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="812" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B812" t="s">
+        <v>129</v>
+      </c>
+      <c r="D812" s="1">
+        <v>49</v>
+      </c>
+      <c r="L812" t="s">
+        <v>194</v>
+      </c>
+      <c r="M812" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="813" spans="2:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="B813" t="s">
+        <v>129</v>
+      </c>
+      <c r="D813" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="L813" t="s">
+        <v>69</v>
+      </c>
+      <c r="N813" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="814" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B814" t="s">
+        <v>129</v>
+      </c>
+      <c r="D814" s="1">
+        <v>51</v>
+      </c>
+      <c r="L814" t="s">
+        <v>194</v>
+      </c>
+      <c r="M814" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="815" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B815" t="s">
+        <v>129</v>
+      </c>
+      <c r="D815" s="1">
+        <v>52</v>
+      </c>
+      <c r="L815" t="s">
+        <v>194</v>
+      </c>
+      <c r="M815" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="816" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B816" t="s">
+        <v>129</v>
+      </c>
+      <c r="D816" s="1">
+        <v>53</v>
+      </c>
+      <c r="L816" t="s">
+        <v>194</v>
+      </c>
+      <c r="M816" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="817" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D817" s="1">
+        <v>54</v>
+      </c>
+      <c r="L817" t="s">
+        <v>194</v>
+      </c>
+      <c r="M817" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="818" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D818" s="1">
+        <v>55</v>
+      </c>
+      <c r="L818" t="s">
+        <v>194</v>
+      </c>
+      <c r="M818" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="819" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D819" s="1">
+        <v>56</v>
+      </c>
+      <c r="L819" t="s">
+        <v>194</v>
+      </c>
+      <c r="M819" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="820" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="D820" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="L820" t="s">
+        <v>69</v>
+      </c>
+      <c r="N820" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="821" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D821" s="1">
+        <v>58</v>
+      </c>
+      <c r="L821" t="s">
+        <v>194</v>
+      </c>
+      <c r="M821" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="822" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="D822" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="L822" t="s">
+        <v>227</v>
+      </c>
+      <c r="N822" t="s">
+        <v>46</v>
+      </c>
+      <c r="O822" t="s">
+        <v>69</v>
+      </c>
+      <c r="P822" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q822" t="s">
+        <v>578</v>
+      </c>
+      <c r="R822" t="s">
+        <v>285</v>
+      </c>
+      <c r="S822" t="s">
+        <v>579</v>
+      </c>
+      <c r="T822">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="823" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D823" s="1">
+        <v>60</v>
+      </c>
+      <c r="L823" t="s">
+        <v>194</v>
+      </c>
+      <c r="M823" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="824" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D824" s="1">
+        <v>61</v>
+      </c>
+      <c r="L824" t="s">
+        <v>194</v>
+      </c>
+      <c r="M824" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="825" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D825" s="1">
+        <v>62</v>
+      </c>
+      <c r="L825" t="s">
+        <v>194</v>
+      </c>
+      <c r="M825" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="826" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D826" s="1">
+        <v>63</v>
+      </c>
+      <c r="L826" t="s">
+        <v>194</v>
+      </c>
+      <c r="M826" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="827" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="D827" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="L827" t="s">
+        <v>69</v>
+      </c>
+      <c r="N827" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="828" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="D828" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="L828" t="s">
+        <v>69</v>
+      </c>
+      <c r="N828" t="s">
+        <v>46</v>
+      </c>
+      <c r="O828" t="s">
+        <v>69</v>
+      </c>
+      <c r="P828" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q828" t="s">
+        <v>582</v>
+      </c>
+      <c r="S828" t="s">
+        <v>583</v>
+      </c>
+      <c r="T828">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="829" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D829" s="1">
+        <v>66</v>
+      </c>
+      <c r="L829" t="s">
+        <v>194</v>
+      </c>
+      <c r="M829" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="830" spans="4:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="D830" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="L830" t="s">
+        <v>227</v>
+      </c>
+      <c r="N830" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="831" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D831" s="1">
+        <v>68</v>
+      </c>
+      <c r="L831" t="s">
+        <v>194</v>
+      </c>
+      <c r="M831" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="832" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="D832" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="L832" t="s">
+        <v>227</v>
+      </c>
+      <c r="N832" t="s">
+        <v>46</v>
+      </c>
+      <c r="O832" t="s">
+        <v>69</v>
+      </c>
+      <c r="P832" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q832" t="s">
+        <v>586</v>
+      </c>
+      <c r="R832" t="s">
+        <v>587</v>
+      </c>
+      <c r="S832" t="s">
+        <v>588</v>
+      </c>
+      <c r="T832">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="833" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D833" s="1">
+        <v>70</v>
+      </c>
+      <c r="L833" t="s">
+        <v>194</v>
+      </c>
+      <c r="M833" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="834" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D834" s="1">
+        <v>71</v>
+      </c>
+      <c r="L834" t="s">
+        <v>194</v>
+      </c>
+      <c r="M834" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="835" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D835" s="1">
+        <v>72</v>
+      </c>
+      <c r="L835" t="s">
+        <v>194</v>
+      </c>
+      <c r="M835" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="836" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D836" s="1">
+        <v>73</v>
+      </c>
+      <c r="L836" t="s">
+        <v>194</v>
+      </c>
+      <c r="M836" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="837" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D837" s="1">
+        <v>74</v>
+      </c>
+      <c r="L837" t="s">
+        <v>194</v>
+      </c>
+      <c r="M837" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="838" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D838" s="1">
+        <v>75</v>
+      </c>
+      <c r="L838" t="s">
+        <v>194</v>
+      </c>
+      <c r="M838" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="839" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D839" s="1">
+        <v>76</v>
+      </c>
+      <c r="L839" t="s">
+        <v>194</v>
+      </c>
+      <c r="M839" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="840" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D840" s="1">
+        <v>77</v>
+      </c>
+      <c r="L840" t="s">
+        <v>194</v>
+      </c>
+      <c r="M840" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="841" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D841" s="1">
+        <v>78</v>
+      </c>
+      <c r="L841" t="s">
+        <v>194</v>
+      </c>
+      <c r="M841" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="842" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D842" s="1">
+        <v>79</v>
+      </c>
+      <c r="L842" t="s">
+        <v>194</v>
+      </c>
+      <c r="M842" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="843" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D843" s="1">
+        <v>80</v>
+      </c>
+      <c r="L843" t="s">
+        <v>194</v>
+      </c>
+      <c r="M843" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="844" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D844" s="1">
+        <v>81</v>
+      </c>
+      <c r="L844" t="s">
+        <v>194</v>
+      </c>
+      <c r="M844" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="845" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D845" s="1">
+        <v>82</v>
+      </c>
+      <c r="L845" t="s">
+        <v>194</v>
+      </c>
+      <c r="M845" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="846" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D846" s="1">
+        <v>83</v>
+      </c>
+      <c r="L846" t="s">
+        <v>194</v>
+      </c>
+      <c r="M846" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="847" spans="4:20" ht="48" x14ac:dyDescent="0.2">
+      <c r="D847" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="L847" t="s">
+        <v>69</v>
+      </c>
+      <c r="N847" t="s">
+        <v>46</v>
+      </c>
+      <c r="O847" t="s">
+        <v>69</v>
+      </c>
+      <c r="P847" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q847" t="s">
+        <v>591</v>
+      </c>
+      <c r="R847" t="s">
+        <v>239</v>
+      </c>
+      <c r="S847" t="s">
+        <v>240</v>
+      </c>
+      <c r="T847">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="848" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D848" s="1">
+        <v>85</v>
+      </c>
+      <c r="L848" t="s">
+        <v>194</v>
+      </c>
+      <c r="M848" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="849" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D849" s="1">
+        <v>86</v>
+      </c>
+      <c r="L849" t="s">
+        <v>194</v>
+      </c>
+      <c r="M849" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="850" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D850" s="1">
+        <v>87</v>
+      </c>
+      <c r="L850" t="s">
+        <v>194</v>
+      </c>
+      <c r="M850" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="851" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D851" s="1">
+        <v>88</v>
+      </c>
+      <c r="L851" t="s">
+        <v>194</v>
+      </c>
+      <c r="M851" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="852" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D852" s="1">
+        <v>89</v>
+      </c>
+      <c r="L852" t="s">
+        <v>194</v>
+      </c>
+      <c r="M852" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="853" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D853" s="1">
+        <v>90</v>
+      </c>
+      <c r="L853" t="s">
+        <v>194</v>
+      </c>
+      <c r="M853" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="854" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D854" s="1">
+        <v>91</v>
+      </c>
+      <c r="L854" t="s">
+        <v>194</v>
+      </c>
+      <c r="M854" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="855" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D855" s="1">
+        <v>92</v>
+      </c>
+      <c r="L855" t="s">
+        <v>194</v>
+      </c>
+      <c r="M855" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="856" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D856" s="1">
+        <v>93</v>
+      </c>
+      <c r="L856" t="s">
+        <v>194</v>
+      </c>
+      <c r="M856" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="857" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D857" s="1">
+        <v>94</v>
+      </c>
+      <c r="L857" t="s">
+        <v>194</v>
+      </c>
+      <c r="M857" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="858" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D858" s="1">
+        <v>95</v>
+      </c>
+      <c r="L858" t="s">
+        <v>194</v>
+      </c>
+      <c r="M858" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="859" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D859" s="1">
+        <v>96</v>
+      </c>
+      <c r="L859" t="s">
+        <v>194</v>
+      </c>
+      <c r="M859" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="860" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="D860" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="L860" t="s">
+        <v>69</v>
+      </c>
+      <c r="N860" t="s">
+        <v>46</v>
+      </c>
+      <c r="O860" t="s">
+        <v>69</v>
+      </c>
+      <c r="P860" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q860" t="s">
+        <v>593</v>
+      </c>
+      <c r="R860" t="s">
+        <v>594</v>
+      </c>
+      <c r="S860" t="s">
+        <v>313</v>
+      </c>
+      <c r="T860">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="861" spans="4:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="D861" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="L861" t="s">
+        <v>227</v>
+      </c>
+      <c r="M861" t="s">
+        <v>470</v>
+      </c>
+      <c r="N861" t="s">
+        <v>194</v>
+      </c>
+      <c r="O861" t="s">
+        <v>227</v>
+      </c>
+      <c r="P861" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q861" t="s">
+        <v>595</v>
+      </c>
+      <c r="S861" t="s">
+        <v>596</v>
+      </c>
+      <c r="T861">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="862" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D862" s="1">
+        <v>99</v>
+      </c>
+      <c r="L862" t="s">
+        <v>194</v>
+      </c>
+      <c r="M862" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="863" spans="4:20" x14ac:dyDescent="0.2">
+      <c r="D863" s="1">
+        <v>100</v>
+      </c>
+      <c r="L863" t="s">
+        <v>194</v>
+      </c>
+      <c r="M863" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>